<commit_message>
plot first motion fall
</commit_message>
<xml_diff>
--- a/fallClean/RaceInfo/Unused_Races.xlsx
+++ b/fallClean/RaceInfo/Unused_Races.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabby/Desktop/dragraceAnalysis-master/fallClean/RaceInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F650BBA3-A90B-FC43-9C50-C36C72568A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA5DB3-C7E6-5642-B3B9-9443276F2089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15940" xr2:uid="{551E6218-B88B-314F-AD4E-DFD86328264C}"/>
+    <workbookView xWindow="13520" yWindow="460" windowWidth="27640" windowHeight="15940" xr2:uid="{551E6218-B88B-314F-AD4E-DFD86328264C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,11 +506,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264BFC7A-AE14-794A-921D-DE84C88B8A07}">
   <dimension ref="A2:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>